<commit_message>
MVC PEMBAYARAN ADM LAIN
</commit_message>
<xml_diff>
--- a/temp_doc/DATA GURU.xlsx
+++ b/temp_doc/DATA GURU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/webth/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE2C5F6-7F9B-5048-AA5C-FA0DCD6EBD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B1BFD8-2E8A-284C-92AE-062AE747E15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{6FC86887-9C03-7848-8C61-7ABDAF95463A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>SWIYONO, SE</t>
   </si>
@@ -106,9 +106,6 @@
     <t>LELY LIANASARI, S.PD</t>
   </si>
   <si>
-    <t>USUP RAHARJO, A.MD</t>
-  </si>
-  <si>
     <t>MUFIDAH, S.E</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>MARIA MENGE, M.PD</t>
   </si>
   <si>
-    <t>RAHMADIKA SURYA S.KOM</t>
-  </si>
-  <si>
     <t>DAYANTI WISNU WARDANI, S.PD</t>
   </si>
   <si>
@@ -181,13 +175,28 @@
     <t>TRIANA SABAWANTI, S.PD</t>
   </si>
   <si>
-    <t>MARCELLINO RADITIO</t>
-  </si>
-  <si>
     <t>DKV</t>
   </si>
   <si>
     <t>ANDIKA</t>
+  </si>
+  <si>
+    <t>KENT PANGESTU</t>
+  </si>
+  <si>
+    <t>TRI FANDI JUNIOR</t>
+  </si>
+  <si>
+    <t>EKA DHANI</t>
+  </si>
+  <si>
+    <t>USUP RAHARJO, S.KOM</t>
+  </si>
+  <si>
+    <t>RAHMADIKA SURYA SETIAWAN, S.KOM</t>
+  </si>
+  <si>
+    <t>MARCELLINO RADITIO, S.KOOM</t>
   </si>
 </sst>
 </file>
@@ -230,10 +239,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2853FF3-1478-2B4F-8C6D-894ED2FC938F}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,468 +569,500 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1001498</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3">
         <v>1002995</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4">
         <v>1003732</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5">
         <v>1004885</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6">
         <v>1005136</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7">
         <v>1006673</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8">
         <v>1007341</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>1008458</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10">
         <v>1009512</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11">
         <v>1010725</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12">
         <v>1011700</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13">
         <v>1012381</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14">
         <v>1013673</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15">
         <v>1014848</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16">
         <v>1015461</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17">
         <v>1016165</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18">
         <v>1017445</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19">
         <v>1018634</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20">
         <v>1019738</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1020859</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>1020859</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22">
         <v>1021895</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23">
         <v>1022279</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24">
         <v>1023816</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25">
         <v>1024870</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26">
         <v>1025999</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27">
         <v>1026111</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
       </c>
       <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1027189</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>1027189</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1028677</v>
+      </c>
+      <c r="B29" t="s">
         <v>22</v>
       </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>1028677</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1029399</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1030373</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1031185</v>
+      </c>
+      <c r="B32" t="s">
         <v>23</v>
       </c>
-      <c r="C29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>1029399</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1032709</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1033114</v>
+      </c>
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1034988</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1035258</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1036320</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1037480</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1038679</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1039813</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1040231</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1041360</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1041361</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1041362</v>
+      </c>
+      <c r="B44" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>1030373</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>1031185</v>
-      </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>1032709</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>1033114</v>
-      </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>1034988</v>
-      </c>
-      <c r="B35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>1035258</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>1036320</v>
-      </c>
-      <c r="B37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>1037480</v>
-      </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>1038679</v>
-      </c>
-      <c r="B39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>1039813</v>
-      </c>
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>1040231</v>
-      </c>
-      <c r="B41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>1041360</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1041363</v>
+      </c>
+      <c r="B45" t="s">
         <v>49</v>
       </c>
-      <c r="C42" t="s">
-        <v>48</v>
+      <c r="C45" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C42" xr:uid="{E2853FF3-1478-2B4F-8C6D-894ED2FC938F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>